<commit_message>
fix testdata inconsistency + allow no CR args
</commit_message>
<xml_diff>
--- a/test/test_sample_info.xlsx
+++ b/test/test_sample_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/mount/snakes/cellrangersnake/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/mount/scratch/projects/cellrangersnake/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D299FB0-076D-9E44-B904-DCEA4ED3EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6662FC9A-AC69-AE4C-9C99-E1D14385D071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="780" windowWidth="20560" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8940" yWindow="780" windowWidth="20560" windowHeight="17620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
     <t>FeatureBarcode</t>
   </si>
   <si>
-    <t>/data/gpfs-1/users/szyskam_c/work/testdata/10x-fastq/cellrangertestdata</t>
+    <t>/data/gpfs-1/users/szyskam_c/scratch/projects/testdata/cellrangertestdata</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
@@ -477,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -636,24 +636,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,10 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -680,17 +659,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +696,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -997,7 +984,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1007,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1027,18 +1014,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
@@ -1272,23 +1259,23 @@
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
       <c r="M1" s="27"/>
       <c r="N1" s="29"/>
     </row>
@@ -1348,7 +1335,7 @@
       <c r="D3" s="50">
         <v>29</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="18" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="18">
@@ -1363,7 +1350,7 @@
       <c r="I3" s="50">
         <v>39</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="J3" s="67" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="18">
@@ -1402,7 +1389,7 @@
       <c r="D5" s="55">
         <v>18</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="6">
@@ -1435,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1FACE-C82F-FA42-88B9-D8C3F5B9E8AE}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,43 +1444,43 @@
       <c r="B1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="24" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="36" t="s">
@@ -1501,35 +1488,35 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="str">
+      <c r="A3" s="58" t="str">
         <f>Status!A3</f>
         <v>LO 009 Tumor</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="65" t="str">
+      <c r="C3" s="59" t="str">
         <f>IF(Status!B3=0,"",Status!B3)</f>
         <v>09T</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="66">
+      <c r="E3" s="60">
         <v>44888</v>
       </c>
-      <c r="F3" s="65">
+      <c r="F3" s="59">
         <f>Status!I3</f>
         <v>3</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="73" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="18">
         <v>0</v>
       </c>
       <c r="I3" s="18"/>
-      <c r="J3" s="67">
+      <c r="J3" s="61">
         <v>0</v>
       </c>
     </row>
@@ -1538,51 +1525,46 @@
         <f>Status!A4</f>
         <v>LO 009 Healthy</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="68" t="str">
+      <c r="C4" s="1" t="str">
         <f>IF(Status!B4=0,"",Status!B4)</f>
         <v/>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="F4" s="62"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="str">
+      <c r="A5" s="63" t="str">
         <f>Status!A5</f>
         <v>LO 009 Tumor organoid WRN</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="71" t="str">
+      <c r="C5" s="64" t="str">
         <f>IF(Status!B5=0,"",Status!B5)</f>
         <v>L09TO</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="65">
         <v>44888</v>
       </c>
-      <c r="F5" s="71">
+      <c r="F5" s="64">
         <f>Status!I5</f>
         <v>4</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="73" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="73">
+      <c r="J5" s="66">
         <v>0</v>
       </c>
     </row>
@@ -1790,26 +1772,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="636018d9-4a34-4186-8868-93b3d1d2bbfb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="509be607-5cb9-4ff6-8f2b-a49830fd41ed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE5F01E4A6836D438E48A173EA646965" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="592d422d8a616dc410bec1c111f87299">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="636018d9-4a34-4186-8868-93b3d1d2bbfb" xmlns:ns3="509be607-5cb9-4ff6-8f2b-a49830fd41ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="980d6db85b21d3dcf27729ecad145c32" ns2:_="" ns3:_="">
     <xsd:import namespace="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
@@ -2040,32 +2002,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1553288E-0F23-412A-BEAB-54B77042EBE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="509be607-5cb9-4ff6-8f2b-a49830fd41ed"/>
-    <ds:schemaRef ds:uri="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB7F689-2F00-463D-9C3A-394EB3DFE7E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="636018d9-4a34-4186-8868-93b3d1d2bbfb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="509be607-5cb9-4ff6-8f2b-a49830fd41ed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10281D8D-E076-42BF-81E5-0FF688BB5245}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2082,4 +2039,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB7F689-2F00-463D-9C3A-394EB3DFE7E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1553288E-0F23-412A-BEAB-54B77042EBE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="509be607-5cb9-4ff6-8f2b-a49830fd41ed"/>
+    <ds:schemaRef ds:uri="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix zero fill in BIMBS ID
</commit_message>
<xml_diff>
--- a/test/test_sample_info.xlsx
+++ b/test/test_sample_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/mount/scratch/projects/cellrangersnake/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6662FC9A-AC69-AE4C-9C99-E1D14385D071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4FAC99-4A75-324D-A82B-CD54E756B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="780" windowWidth="20560" windowHeight="17620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8940" yWindow="780" windowWidth="20560" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -662,6 +662,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,7 +678,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,18 +1014,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,23 +1259,23 @@
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
       <c r="M1" s="27"/>
       <c r="N1" s="29"/>
     </row>
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1FACE-C82F-FA42-88B9-D8C3F5B9E8AE}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,16 +1444,16 @@
       <c r="B1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="70"/>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
@@ -1509,7 +1509,7 @@
         <f>Status!I3</f>
         <v>3</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="G3" s="68" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="18">
@@ -1557,7 +1557,7 @@
         <f>Status!I5</f>
         <v>4</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="68" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="6">
@@ -1772,6 +1772,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="636018d9-4a34-4186-8868-93b3d1d2bbfb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="509be607-5cb9-4ff6-8f2b-a49830fd41ed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE5F01E4A6836D438E48A173EA646965" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="592d422d8a616dc410bec1c111f87299">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="636018d9-4a34-4186-8868-93b3d1d2bbfb" xmlns:ns3="509be607-5cb9-4ff6-8f2b-a49830fd41ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="980d6db85b21d3dcf27729ecad145c32" ns2:_="" ns3:_="">
     <xsd:import namespace="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
@@ -2002,27 +2022,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1553288E-0F23-412A-BEAB-54B77042EBE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="509be607-5cb9-4ff6-8f2b-a49830fd41ed"/>
+    <ds:schemaRef ds:uri="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="636018d9-4a34-4186-8868-93b3d1d2bbfb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="509be607-5cb9-4ff6-8f2b-a49830fd41ed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB7F689-2F00-463D-9C3A-394EB3DFE7E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10281D8D-E076-42BF-81E5-0FF688BB5245}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2039,29 +2064,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB7F689-2F00-463D-9C3A-394EB3DFE7E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1553288E-0F23-412A-BEAB-54B77042EBE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="509be607-5cb9-4ff6-8f2b-a49830fd41ed"/>
-    <ds:schemaRef ds:uri="636018d9-4a34-4186-8868-93b3d1d2bbfb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>